<commit_message>
SERVICES API WITH AUTH
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABSEN EKINERJA\08. ABSEN Agustus 20 22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABSEN EKINERJA\09. ABSEN September 22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E751C93E-A1AB-49AD-8C3D-F5D375AB9C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD304297-195D-4166-A80D-5919D1829035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nov (4)" sheetId="4" state="hidden" r:id="rId1"/>
-    <sheet name="agustus" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="september" sheetId="1" r:id="rId2"/>
+    <sheet name="september (2)" sheetId="7" r:id="rId3"/>
+    <sheet name="Juli (2)" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="245">
   <si>
     <t>NIP</t>
   </si>
@@ -760,6 +762,12 @@
   </si>
   <si>
     <t>YUDIANNOR</t>
+  </si>
+  <si>
+    <t>SDN GELUMBANG JUAI</t>
+  </si>
+  <si>
+    <t>DAFTAR YANG BELUM MENYAMPAIKAN ABSENSI TPP BULAN JULI 2022</t>
   </si>
 </sst>
 </file>
@@ -844,7 +852,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -871,7 +879,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -951,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1013,27 +1039,101 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4535,9 +4635,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4545,9 +4647,10 @@
     <col min="2" max="3" width="9.7265625" customWidth="1"/>
     <col min="4" max="5" width="12.26953125" customWidth="1"/>
     <col min="6" max="6" width="21.26953125" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4567,1421 +4670,1426 @@
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="31">
-        <v>8</v>
-      </c>
-      <c r="C2" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D2" s="31">
-        <v>26</v>
-      </c>
-      <c r="E2" s="31">
-        <v>26</v>
-      </c>
-      <c r="F2" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
+      <c r="B2" s="60">
+        <v>9</v>
+      </c>
+      <c r="C2" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="60">
+        <v>26</v>
+      </c>
+      <c r="E2" s="60">
+        <v>26</v>
+      </c>
+      <c r="F2" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="66" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="31">
-        <v>8</v>
-      </c>
-      <c r="C3" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D3" s="31">
-        <v>26</v>
-      </c>
-      <c r="E3" s="31">
-        <v>26</v>
-      </c>
-      <c r="F3" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
+      <c r="B3" s="60">
+        <v>9</v>
+      </c>
+      <c r="C3" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D3" s="60">
+        <v>26</v>
+      </c>
+      <c r="E3" s="60">
+        <v>26</v>
+      </c>
+      <c r="F3" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="66" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="31">
-        <v>8</v>
-      </c>
-      <c r="C4" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D4" s="31">
-        <v>26</v>
-      </c>
-      <c r="E4" s="31">
-        <v>26</v>
-      </c>
-      <c r="F4" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33" t="s">
+      <c r="B4" s="60">
+        <v>9</v>
+      </c>
+      <c r="C4" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D4" s="60">
+        <v>26</v>
+      </c>
+      <c r="E4" s="60">
+        <v>26</v>
+      </c>
+      <c r="F4" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="31">
-        <v>8</v>
-      </c>
-      <c r="C5" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D5" s="31">
-        <v>26</v>
-      </c>
-      <c r="E5" s="31">
-        <v>26</v>
-      </c>
-      <c r="F5" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="30" t="s">
+      <c r="B5" s="60">
+        <v>9</v>
+      </c>
+      <c r="C5" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D5" s="60">
+        <v>26</v>
+      </c>
+      <c r="E5" s="60">
+        <v>26</v>
+      </c>
+      <c r="F5" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="31">
-        <v>8</v>
-      </c>
-      <c r="C6" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D6" s="31">
-        <v>26</v>
-      </c>
-      <c r="E6" s="31">
-        <v>26</v>
-      </c>
-      <c r="F6" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+      <c r="B6" s="60">
+        <v>9</v>
+      </c>
+      <c r="C6" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D6" s="60">
+        <v>26</v>
+      </c>
+      <c r="E6" s="60">
+        <v>26</v>
+      </c>
+      <c r="F6" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="31">
-        <v>8</v>
-      </c>
-      <c r="C7" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D7" s="31">
-        <v>26</v>
-      </c>
-      <c r="E7" s="31">
-        <v>26</v>
-      </c>
-      <c r="F7" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
+      <c r="B7" s="60">
+        <v>9</v>
+      </c>
+      <c r="C7" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D7" s="60">
+        <v>26</v>
+      </c>
+      <c r="E7" s="60">
+        <v>26</v>
+      </c>
+      <c r="F7" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="59" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="31">
-        <v>8</v>
-      </c>
-      <c r="C8" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D8" s="31">
-        <v>26</v>
-      </c>
-      <c r="E8" s="31">
-        <v>26</v>
-      </c>
-      <c r="F8" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
+      <c r="B8" s="60">
+        <v>9</v>
+      </c>
+      <c r="C8" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D8" s="60">
+        <v>26</v>
+      </c>
+      <c r="E8" s="60">
+        <v>26</v>
+      </c>
+      <c r="F8" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="B9" s="31">
-        <v>8</v>
-      </c>
-      <c r="C9" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D9" s="31">
-        <v>26</v>
-      </c>
-      <c r="E9" s="31">
-        <v>26</v>
-      </c>
-      <c r="F9" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="34" t="s">
+      <c r="B9" s="60">
+        <v>9</v>
+      </c>
+      <c r="C9" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="60">
+        <v>26</v>
+      </c>
+      <c r="E9" s="60">
+        <v>26</v>
+      </c>
+      <c r="F9" s="60">
+        <v>0</v>
+      </c>
+      <c r="G9" s="61"/>
+    </row>
+    <row r="10" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="31">
-        <v>8</v>
-      </c>
-      <c r="C10" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D10" s="31">
-        <v>26</v>
-      </c>
-      <c r="E10" s="31">
-        <v>26</v>
-      </c>
-      <c r="F10" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="30" t="s">
+      <c r="B10" s="60">
+        <v>9</v>
+      </c>
+      <c r="C10" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D10" s="60">
+        <v>26</v>
+      </c>
+      <c r="E10" s="60">
+        <v>26</v>
+      </c>
+      <c r="F10" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="59" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="31">
-        <v>8</v>
-      </c>
-      <c r="C11" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D11" s="31">
-        <v>26</v>
-      </c>
-      <c r="E11" s="31">
-        <v>26</v>
-      </c>
-      <c r="F11" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
+      <c r="B11" s="60">
+        <v>9</v>
+      </c>
+      <c r="C11" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D11" s="60">
+        <v>26</v>
+      </c>
+      <c r="E11" s="60">
+        <v>26</v>
+      </c>
+      <c r="F11" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="B12" s="31">
-        <v>8</v>
-      </c>
-      <c r="C12" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D12" s="31">
-        <v>26</v>
-      </c>
-      <c r="E12" s="31">
-        <v>26</v>
-      </c>
-      <c r="F12" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="30" t="s">
+      <c r="B12" s="60">
+        <v>9</v>
+      </c>
+      <c r="C12" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D12" s="60">
+        <v>26</v>
+      </c>
+      <c r="E12" s="60">
+        <v>26</v>
+      </c>
+      <c r="F12" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="31">
-        <v>8</v>
-      </c>
-      <c r="C13" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D13" s="31">
-        <v>26</v>
-      </c>
-      <c r="E13" s="31">
-        <v>26</v>
-      </c>
-      <c r="F13" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+      <c r="B13" s="60">
+        <v>9</v>
+      </c>
+      <c r="C13" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D13" s="60">
+        <v>26</v>
+      </c>
+      <c r="E13" s="60">
+        <v>26</v>
+      </c>
+      <c r="F13" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="31">
-        <v>8</v>
-      </c>
-      <c r="C14" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D14" s="31">
-        <v>26</v>
-      </c>
-      <c r="E14" s="31">
-        <v>26</v>
-      </c>
-      <c r="F14" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="30" t="s">
+      <c r="B14" s="60">
+        <v>9</v>
+      </c>
+      <c r="C14" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D14" s="60">
+        <v>26</v>
+      </c>
+      <c r="E14" s="60">
+        <v>26</v>
+      </c>
+      <c r="F14" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="59" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="31">
-        <v>8</v>
-      </c>
-      <c r="C15" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D15" s="31">
-        <v>26</v>
-      </c>
-      <c r="E15" s="31">
-        <v>26</v>
-      </c>
-      <c r="F15" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="30" t="s">
+      <c r="B15" s="60">
+        <v>9</v>
+      </c>
+      <c r="C15" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D15" s="60">
+        <v>26</v>
+      </c>
+      <c r="E15" s="60">
+        <v>26</v>
+      </c>
+      <c r="F15" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="B16" s="31">
-        <v>8</v>
-      </c>
-      <c r="C16" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D16" s="31">
-        <v>26</v>
-      </c>
-      <c r="E16" s="31">
-        <v>26</v>
-      </c>
-      <c r="F16" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="30" t="s">
+      <c r="B16" s="60">
+        <v>9</v>
+      </c>
+      <c r="C16" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D16" s="60">
+        <v>26</v>
+      </c>
+      <c r="E16" s="60">
+        <v>26</v>
+      </c>
+      <c r="F16" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="59" t="s">
         <v>175</v>
       </c>
-      <c r="B17" s="31">
-        <v>8</v>
-      </c>
-      <c r="C17" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D17" s="31">
-        <v>26</v>
-      </c>
-      <c r="E17" s="31">
-        <v>26</v>
-      </c>
-      <c r="F17" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="30" t="s">
+      <c r="B17" s="60">
+        <v>9</v>
+      </c>
+      <c r="C17" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D17" s="60">
+        <v>26</v>
+      </c>
+      <c r="E17" s="60">
+        <v>26</v>
+      </c>
+      <c r="F17" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="B18" s="31">
-        <v>8</v>
-      </c>
-      <c r="C18" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D18" s="31">
-        <v>26</v>
-      </c>
-      <c r="E18" s="31">
-        <v>26</v>
-      </c>
-      <c r="F18" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="30" t="s">
+      <c r="B18" s="60">
+        <v>9</v>
+      </c>
+      <c r="C18" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D18" s="60">
+        <v>26</v>
+      </c>
+      <c r="E18" s="60">
+        <v>26</v>
+      </c>
+      <c r="F18" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="B19" s="31">
-        <v>8</v>
-      </c>
-      <c r="C19" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D19" s="31">
-        <v>26</v>
-      </c>
-      <c r="E19" s="31">
-        <v>26</v>
-      </c>
-      <c r="F19" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="30" t="s">
+      <c r="B19" s="60">
+        <v>9</v>
+      </c>
+      <c r="C19" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D19" s="60">
+        <v>26</v>
+      </c>
+      <c r="E19" s="60">
+        <v>26</v>
+      </c>
+      <c r="F19" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="B20" s="31">
-        <v>8</v>
-      </c>
-      <c r="C20" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D20" s="31">
-        <v>26</v>
-      </c>
-      <c r="E20" s="31">
-        <v>26</v>
-      </c>
-      <c r="F20" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="30" t="s">
+      <c r="B20" s="60">
+        <v>9</v>
+      </c>
+      <c r="C20" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D20" s="60">
+        <v>26</v>
+      </c>
+      <c r="E20" s="60">
+        <v>26</v>
+      </c>
+      <c r="F20" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="B21" s="31">
-        <v>8</v>
-      </c>
-      <c r="C21" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D21" s="31">
-        <v>26</v>
-      </c>
-      <c r="E21" s="31">
-        <v>26</v>
-      </c>
-      <c r="F21" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="30" t="s">
+      <c r="B21" s="60">
+        <v>9</v>
+      </c>
+      <c r="C21" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D21" s="60">
+        <v>26</v>
+      </c>
+      <c r="E21" s="60">
+        <v>26</v>
+      </c>
+      <c r="F21" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="31">
-        <v>8</v>
-      </c>
-      <c r="C22" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D22" s="31">
-        <v>26</v>
-      </c>
-      <c r="E22" s="31">
-        <v>26</v>
-      </c>
-      <c r="F22" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="30" t="s">
+      <c r="B22" s="60">
+        <v>9</v>
+      </c>
+      <c r="C22" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D22" s="60">
+        <v>26</v>
+      </c>
+      <c r="E22" s="60">
+        <v>26</v>
+      </c>
+      <c r="F22" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="59" t="s">
         <v>207</v>
       </c>
-      <c r="B23" s="31">
-        <v>8</v>
-      </c>
-      <c r="C23" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D23" s="31">
-        <v>26</v>
-      </c>
-      <c r="E23" s="31">
-        <v>26</v>
-      </c>
-      <c r="F23" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="30" t="s">
+      <c r="B23" s="60">
+        <v>9</v>
+      </c>
+      <c r="C23" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D23" s="60">
+        <v>26</v>
+      </c>
+      <c r="E23" s="60">
+        <v>26</v>
+      </c>
+      <c r="F23" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="59" t="s">
         <v>198</v>
       </c>
-      <c r="B24" s="31">
-        <v>8</v>
-      </c>
-      <c r="C24" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D24" s="31">
-        <v>26</v>
-      </c>
-      <c r="E24" s="31">
-        <v>26</v>
-      </c>
-      <c r="F24" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="30" t="s">
+      <c r="B24" s="60">
+        <v>9</v>
+      </c>
+      <c r="C24" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D24" s="60">
+        <v>26</v>
+      </c>
+      <c r="E24" s="60">
+        <v>26</v>
+      </c>
+      <c r="F24" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="59" t="s">
         <v>203</v>
       </c>
-      <c r="B25" s="31">
-        <v>8</v>
-      </c>
-      <c r="C25" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D25" s="31">
-        <v>26</v>
-      </c>
-      <c r="E25" s="31">
-        <v>26</v>
-      </c>
-      <c r="F25" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="30" t="s">
+      <c r="B25" s="60">
+        <v>9</v>
+      </c>
+      <c r="C25" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D25" s="60">
+        <v>26</v>
+      </c>
+      <c r="E25" s="60">
+        <v>26</v>
+      </c>
+      <c r="F25" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="B26" s="31">
-        <v>8</v>
-      </c>
-      <c r="C26" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D26" s="31">
-        <v>26</v>
-      </c>
-      <c r="E26" s="31">
-        <v>26</v>
-      </c>
-      <c r="F26" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="35" t="s">
+      <c r="B26" s="60">
+        <v>9</v>
+      </c>
+      <c r="C26" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="60">
+        <v>26</v>
+      </c>
+      <c r="E26" s="60">
+        <v>26</v>
+      </c>
+      <c r="F26" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="63" t="s">
         <v>177</v>
       </c>
-      <c r="B27" s="31">
-        <v>8</v>
-      </c>
-      <c r="C27" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D27" s="31">
-        <v>26</v>
-      </c>
-      <c r="E27" s="31">
-        <v>26</v>
-      </c>
-      <c r="F27" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="35" t="s">
+      <c r="B27" s="60">
+        <v>9</v>
+      </c>
+      <c r="C27" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D27" s="60">
+        <v>26</v>
+      </c>
+      <c r="E27" s="60">
+        <v>26</v>
+      </c>
+      <c r="F27" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="B28" s="31">
-        <v>8</v>
-      </c>
-      <c r="C28" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D28" s="31">
-        <v>26</v>
-      </c>
-      <c r="E28" s="31">
-        <v>26</v>
-      </c>
-      <c r="F28" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="35" t="s">
+      <c r="B28" s="60">
+        <v>9</v>
+      </c>
+      <c r="C28" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D28" s="60">
+        <v>26</v>
+      </c>
+      <c r="E28" s="60">
+        <v>26</v>
+      </c>
+      <c r="F28" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="63" t="s">
         <v>179</v>
       </c>
-      <c r="B29" s="31">
-        <v>8</v>
-      </c>
-      <c r="C29" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D29" s="31">
-        <v>26</v>
-      </c>
-      <c r="E29" s="31">
-        <v>26</v>
-      </c>
-      <c r="F29" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30" t="s">
+      <c r="B29" s="60">
+        <v>9</v>
+      </c>
+      <c r="C29" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D29" s="60">
+        <v>26</v>
+      </c>
+      <c r="E29" s="60">
+        <v>26</v>
+      </c>
+      <c r="F29" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="B30" s="31">
-        <v>8</v>
-      </c>
-      <c r="C30" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D30" s="31">
-        <v>26</v>
-      </c>
-      <c r="E30" s="31">
-        <v>26</v>
-      </c>
-      <c r="F30" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="30" t="s">
+      <c r="B30" s="60">
+        <v>9</v>
+      </c>
+      <c r="C30" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D30" s="60">
+        <v>26</v>
+      </c>
+      <c r="E30" s="60">
+        <v>26</v>
+      </c>
+      <c r="F30" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="B31" s="31">
-        <v>8</v>
-      </c>
-      <c r="C31" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D31" s="31">
-        <v>26</v>
-      </c>
-      <c r="E31" s="31">
-        <v>26</v>
-      </c>
-      <c r="F31" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="30" t="s">
+      <c r="B31" s="60">
+        <v>9</v>
+      </c>
+      <c r="C31" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D31" s="60">
+        <v>26</v>
+      </c>
+      <c r="E31" s="60">
+        <v>26</v>
+      </c>
+      <c r="F31" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="B32" s="31">
-        <v>8</v>
-      </c>
-      <c r="C32" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D32" s="31">
-        <v>26</v>
-      </c>
-      <c r="E32" s="31">
-        <v>26</v>
-      </c>
-      <c r="F32" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="30" t="s">
+      <c r="B32" s="60">
+        <v>9</v>
+      </c>
+      <c r="C32" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D32" s="60">
+        <v>26</v>
+      </c>
+      <c r="E32" s="60">
+        <v>26</v>
+      </c>
+      <c r="F32" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="B33" s="31">
-        <v>8</v>
-      </c>
-      <c r="C33" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D33" s="31">
-        <v>26</v>
-      </c>
-      <c r="E33" s="31">
-        <v>26</v>
-      </c>
-      <c r="F33" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="30" t="s">
+      <c r="B33" s="60">
+        <v>9</v>
+      </c>
+      <c r="C33" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D33" s="60">
+        <v>26</v>
+      </c>
+      <c r="E33" s="60">
+        <v>26</v>
+      </c>
+      <c r="F33" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="B34" s="31">
-        <v>8</v>
-      </c>
-      <c r="C34" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D34" s="31">
-        <v>26</v>
-      </c>
-      <c r="E34" s="31">
-        <v>26</v>
-      </c>
-      <c r="F34" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="30" t="s">
+      <c r="B34" s="60">
+        <v>9</v>
+      </c>
+      <c r="C34" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D34" s="60">
+        <v>26</v>
+      </c>
+      <c r="E34" s="60">
+        <v>26</v>
+      </c>
+      <c r="F34" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="59" t="s">
         <v>205</v>
       </c>
-      <c r="B35" s="31">
-        <v>8</v>
-      </c>
-      <c r="C35" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D35" s="31">
-        <v>26</v>
-      </c>
-      <c r="E35" s="31">
-        <v>26</v>
-      </c>
-      <c r="F35" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="30" t="s">
+      <c r="B35" s="60">
+        <v>9</v>
+      </c>
+      <c r="C35" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D35" s="60">
+        <v>26</v>
+      </c>
+      <c r="E35" s="60">
+        <v>26</v>
+      </c>
+      <c r="F35" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="B36" s="31">
-        <v>8</v>
-      </c>
-      <c r="C36" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D36" s="31">
-        <v>26</v>
-      </c>
-      <c r="E36" s="31">
-        <v>26</v>
-      </c>
-      <c r="F36" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="30" t="s">
+      <c r="B36" s="60">
+        <v>9</v>
+      </c>
+      <c r="C36" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D36" s="60">
+        <v>26</v>
+      </c>
+      <c r="E36" s="60">
+        <v>26</v>
+      </c>
+      <c r="F36" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="59" t="s">
         <v>200</v>
       </c>
-      <c r="B37" s="31">
-        <v>8</v>
-      </c>
-      <c r="C37" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D37" s="31">
-        <v>26</v>
-      </c>
-      <c r="E37" s="31">
-        <v>26</v>
-      </c>
-      <c r="F37" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="30" t="s">
+      <c r="B37" s="60">
+        <v>9</v>
+      </c>
+      <c r="C37" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D37" s="60">
+        <v>26</v>
+      </c>
+      <c r="E37" s="60">
+        <v>26</v>
+      </c>
+      <c r="F37" s="60">
+        <v>0</v>
+      </c>
+      <c r="G37" s="61"/>
+    </row>
+    <row r="38" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="B38" s="31">
-        <v>8</v>
-      </c>
-      <c r="C38" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D38" s="31">
-        <v>26</v>
-      </c>
-      <c r="E38" s="31">
-        <v>26</v>
-      </c>
-      <c r="F38" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="30" t="s">
+      <c r="B38" s="60">
+        <v>9</v>
+      </c>
+      <c r="C38" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D38" s="60">
+        <v>26</v>
+      </c>
+      <c r="E38" s="60">
+        <v>26</v>
+      </c>
+      <c r="F38" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="59" t="s">
         <v>206</v>
       </c>
-      <c r="B39" s="31">
-        <v>8</v>
-      </c>
-      <c r="C39" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D39" s="31">
-        <v>26</v>
-      </c>
-      <c r="E39" s="31">
-        <v>26</v>
-      </c>
-      <c r="F39" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="30" t="s">
+      <c r="B39" s="60">
+        <v>9</v>
+      </c>
+      <c r="C39" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D39" s="60">
+        <v>26</v>
+      </c>
+      <c r="E39" s="60">
+        <v>26</v>
+      </c>
+      <c r="F39" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="B40" s="31">
-        <v>8</v>
-      </c>
-      <c r="C40" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D40" s="31">
-        <v>26</v>
-      </c>
-      <c r="E40" s="31">
-        <v>26</v>
-      </c>
-      <c r="F40" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="30" t="s">
+      <c r="B40" s="60">
+        <v>9</v>
+      </c>
+      <c r="C40" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D40" s="60">
+        <v>26</v>
+      </c>
+      <c r="E40" s="60">
+        <v>26</v>
+      </c>
+      <c r="F40" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="59" t="s">
         <v>211</v>
       </c>
-      <c r="B41" s="31">
-        <v>8</v>
-      </c>
-      <c r="C41" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D41" s="31">
-        <v>26</v>
-      </c>
-      <c r="E41" s="31">
-        <v>26</v>
-      </c>
-      <c r="F41" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="30" t="s">
+      <c r="B41" s="60">
+        <v>9</v>
+      </c>
+      <c r="C41" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D41" s="60">
+        <v>26</v>
+      </c>
+      <c r="E41" s="60">
+        <v>26</v>
+      </c>
+      <c r="F41" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="59" t="s">
         <v>194</v>
       </c>
-      <c r="B42" s="31">
-        <v>8</v>
-      </c>
-      <c r="C42" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D42" s="31">
-        <v>26</v>
-      </c>
-      <c r="E42" s="31">
-        <v>26</v>
-      </c>
-      <c r="F42" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="30" t="s">
+      <c r="B42" s="60">
+        <v>9</v>
+      </c>
+      <c r="C42" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D42" s="60">
+        <v>26</v>
+      </c>
+      <c r="E42" s="60">
+        <v>26</v>
+      </c>
+      <c r="F42" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="59" t="s">
         <v>192</v>
       </c>
-      <c r="B43" s="31">
-        <v>8</v>
-      </c>
-      <c r="C43" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D43" s="31">
-        <v>26</v>
-      </c>
-      <c r="E43" s="31">
-        <v>26</v>
-      </c>
-      <c r="F43" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="30" t="s">
+      <c r="B43" s="60">
+        <v>9</v>
+      </c>
+      <c r="C43" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D43" s="60">
+        <v>26</v>
+      </c>
+      <c r="E43" s="60">
+        <v>26</v>
+      </c>
+      <c r="F43" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="59" t="s">
         <v>189</v>
       </c>
-      <c r="B44" s="31">
-        <v>8</v>
-      </c>
-      <c r="C44" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D44" s="31">
-        <v>26</v>
-      </c>
-      <c r="E44" s="31">
-        <v>26</v>
-      </c>
-      <c r="F44" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="30" t="s">
+      <c r="B44" s="60">
+        <v>9</v>
+      </c>
+      <c r="C44" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D44" s="60">
+        <v>26</v>
+      </c>
+      <c r="E44" s="60">
+        <v>26</v>
+      </c>
+      <c r="F44" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="B45" s="31">
-        <v>8</v>
-      </c>
-      <c r="C45" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D45" s="31">
-        <v>26</v>
-      </c>
-      <c r="E45" s="31">
-        <v>26</v>
-      </c>
-      <c r="F45" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="30" t="s">
+      <c r="B45" s="60">
+        <v>9</v>
+      </c>
+      <c r="C45" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D45" s="60">
+        <v>26</v>
+      </c>
+      <c r="E45" s="60">
+        <v>26</v>
+      </c>
+      <c r="F45" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="59" t="s">
         <v>241</v>
       </c>
-      <c r="B46" s="31">
-        <v>8</v>
-      </c>
-      <c r="C46" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D46" s="31">
-        <v>26</v>
-      </c>
-      <c r="E46" s="31">
-        <v>26</v>
-      </c>
-      <c r="F46" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="30" t="s">
+      <c r="B46" s="60">
+        <v>9</v>
+      </c>
+      <c r="C46" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D46" s="60">
+        <v>26</v>
+      </c>
+      <c r="E46" s="60">
+        <v>26</v>
+      </c>
+      <c r="F46" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="59" t="s">
         <v>152</v>
       </c>
-      <c r="B47" s="31">
-        <v>8</v>
-      </c>
-      <c r="C47" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D47" s="31">
-        <v>26</v>
-      </c>
-      <c r="E47" s="31">
-        <v>26</v>
-      </c>
-      <c r="F47" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="30" t="s">
+      <c r="B47" s="60">
+        <v>9</v>
+      </c>
+      <c r="C47" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D47" s="60">
+        <v>26</v>
+      </c>
+      <c r="E47" s="60">
+        <v>26</v>
+      </c>
+      <c r="F47" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="B48" s="31">
-        <v>8</v>
-      </c>
-      <c r="C48" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D48" s="31">
-        <v>26</v>
-      </c>
-      <c r="E48" s="31">
-        <v>26</v>
-      </c>
-      <c r="F48" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="30" t="s">
+      <c r="B48" s="60">
+        <v>9</v>
+      </c>
+      <c r="C48" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D48" s="60">
+        <v>26</v>
+      </c>
+      <c r="E48" s="60">
+        <v>26</v>
+      </c>
+      <c r="F48" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="B49" s="31">
-        <v>8</v>
-      </c>
-      <c r="C49" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D49" s="31">
-        <v>26</v>
-      </c>
-      <c r="E49" s="31">
-        <v>26</v>
-      </c>
-      <c r="F49" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="30" t="s">
+      <c r="B49" s="60">
+        <v>9</v>
+      </c>
+      <c r="C49" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D49" s="60">
+        <v>26</v>
+      </c>
+      <c r="E49" s="60">
+        <v>26</v>
+      </c>
+      <c r="F49" s="60">
+        <v>0</v>
+      </c>
+      <c r="G49" s="61"/>
+    </row>
+    <row r="50" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="B50" s="31">
-        <v>8</v>
-      </c>
-      <c r="C50" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D50" s="31">
-        <v>26</v>
-      </c>
-      <c r="E50" s="31">
-        <v>26</v>
-      </c>
-      <c r="F50" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="30" t="s">
+      <c r="B50" s="60">
+        <v>9</v>
+      </c>
+      <c r="C50" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D50" s="60">
+        <v>26</v>
+      </c>
+      <c r="E50" s="60">
+        <v>26</v>
+      </c>
+      <c r="F50" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="B51" s="31">
-        <v>8</v>
-      </c>
-      <c r="C51" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D51" s="31">
-        <v>26</v>
-      </c>
-      <c r="E51" s="31">
-        <v>26</v>
-      </c>
-      <c r="F51" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="30" t="s">
+      <c r="B51" s="60">
+        <v>9</v>
+      </c>
+      <c r="C51" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D51" s="60">
+        <v>26</v>
+      </c>
+      <c r="E51" s="60">
+        <v>26</v>
+      </c>
+      <c r="F51" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="B52" s="31">
-        <v>8</v>
-      </c>
-      <c r="C52" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D52" s="31">
-        <v>26</v>
-      </c>
-      <c r="E52" s="31">
-        <v>26</v>
-      </c>
-      <c r="F52" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="30" t="s">
+      <c r="B52" s="60">
+        <v>9</v>
+      </c>
+      <c r="C52" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D52" s="60">
+        <v>26</v>
+      </c>
+      <c r="E52" s="60">
+        <v>26</v>
+      </c>
+      <c r="F52" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="B53" s="31">
-        <v>8</v>
-      </c>
-      <c r="C53" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D53" s="31">
-        <v>26</v>
-      </c>
-      <c r="E53" s="31">
-        <v>26</v>
-      </c>
-      <c r="F53" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="30" t="s">
+      <c r="B53" s="60">
+        <v>9</v>
+      </c>
+      <c r="C53" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D53" s="60">
+        <v>26</v>
+      </c>
+      <c r="E53" s="60">
+        <v>26</v>
+      </c>
+      <c r="F53" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="B54" s="31">
-        <v>8</v>
-      </c>
-      <c r="C54" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D54" s="31">
-        <v>26</v>
-      </c>
-      <c r="E54" s="31">
-        <v>26</v>
-      </c>
-      <c r="F54" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="30" t="s">
+      <c r="B54" s="60">
+        <v>9</v>
+      </c>
+      <c r="C54" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D54" s="60">
+        <v>26</v>
+      </c>
+      <c r="E54" s="60">
+        <v>26</v>
+      </c>
+      <c r="F54" s="60">
+        <v>0</v>
+      </c>
+      <c r="G54" s="65"/>
+    </row>
+    <row r="55" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="59" t="s">
         <v>187</v>
       </c>
-      <c r="B55" s="31">
-        <v>8</v>
-      </c>
-      <c r="C55" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D55" s="31">
-        <v>26</v>
-      </c>
-      <c r="E55" s="31">
-        <v>26</v>
-      </c>
-      <c r="F55" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="30" t="s">
+      <c r="B55" s="60">
+        <v>9</v>
+      </c>
+      <c r="C55" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D55" s="60">
+        <v>26</v>
+      </c>
+      <c r="E55" s="60">
+        <v>26</v>
+      </c>
+      <c r="F55" s="60">
+        <v>0</v>
+      </c>
+      <c r="G55" s="65"/>
+    </row>
+    <row r="56" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="B56" s="31">
-        <v>8</v>
-      </c>
-      <c r="C56" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D56" s="31">
-        <v>26</v>
-      </c>
-      <c r="E56" s="31">
-        <v>26</v>
-      </c>
-      <c r="F56" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="36" t="s">
+      <c r="B56" s="60">
+        <v>9</v>
+      </c>
+      <c r="C56" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D56" s="60">
+        <v>26</v>
+      </c>
+      <c r="E56" s="60">
+        <v>26</v>
+      </c>
+      <c r="F56" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="67" t="s">
         <v>210</v>
       </c>
-      <c r="B57" s="31">
-        <v>8</v>
-      </c>
-      <c r="C57" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D57" s="31">
-        <v>26</v>
-      </c>
-      <c r="E57" s="31">
-        <v>26</v>
-      </c>
-      <c r="F57" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="30" t="s">
+      <c r="B57" s="60">
+        <v>9</v>
+      </c>
+      <c r="C57" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D57" s="60">
+        <v>26</v>
+      </c>
+      <c r="E57" s="60">
+        <v>26</v>
+      </c>
+      <c r="F57" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="59" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="31">
-        <v>8</v>
-      </c>
-      <c r="C58" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D58" s="31">
-        <v>26</v>
-      </c>
-      <c r="E58" s="31">
-        <v>26</v>
-      </c>
-      <c r="F58" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="30" t="s">
+      <c r="B58" s="60">
+        <v>9</v>
+      </c>
+      <c r="C58" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D58" s="60">
+        <v>26</v>
+      </c>
+      <c r="E58" s="60">
+        <v>26</v>
+      </c>
+      <c r="F58" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="B59" s="31">
-        <v>8</v>
-      </c>
-      <c r="C59" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D59" s="31">
-        <v>26</v>
-      </c>
-      <c r="E59" s="31">
-        <v>26</v>
-      </c>
-      <c r="F59" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="30" t="s">
+      <c r="B59" s="60">
+        <v>9</v>
+      </c>
+      <c r="C59" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D59" s="60">
+        <v>26</v>
+      </c>
+      <c r="E59" s="60">
+        <v>26</v>
+      </c>
+      <c r="F59" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="B60" s="31">
-        <v>8</v>
-      </c>
-      <c r="C60" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D60" s="31">
-        <v>26</v>
-      </c>
-      <c r="E60" s="31">
-        <v>26</v>
-      </c>
-      <c r="F60" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="30" t="s">
+      <c r="B60" s="60">
+        <v>9</v>
+      </c>
+      <c r="C60" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D60" s="60">
+        <v>26</v>
+      </c>
+      <c r="E60" s="60">
+        <v>26</v>
+      </c>
+      <c r="F60" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="B61" s="31">
-        <v>8</v>
-      </c>
-      <c r="C61" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D61" s="31">
-        <v>26</v>
-      </c>
-      <c r="E61" s="31">
-        <v>26</v>
-      </c>
-      <c r="F61" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="30" t="s">
+      <c r="B61" s="60">
+        <v>9</v>
+      </c>
+      <c r="C61" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D61" s="60">
+        <v>26</v>
+      </c>
+      <c r="E61" s="60">
+        <v>26</v>
+      </c>
+      <c r="F61" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="59" t="s">
         <v>208</v>
       </c>
-      <c r="B62" s="31">
-        <v>8</v>
-      </c>
-      <c r="C62" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D62" s="31">
-        <v>26</v>
-      </c>
-      <c r="E62" s="31">
-        <v>26</v>
-      </c>
-      <c r="F62" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="30" t="s">
+      <c r="B62" s="60">
+        <v>9</v>
+      </c>
+      <c r="C62" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D62" s="60">
+        <v>26</v>
+      </c>
+      <c r="E62" s="60">
+        <v>26</v>
+      </c>
+      <c r="F62" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="59" t="s">
         <v>204</v>
       </c>
-      <c r="B63" s="31">
-        <v>8</v>
-      </c>
-      <c r="C63" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D63" s="31">
-        <v>26</v>
-      </c>
-      <c r="E63" s="31">
-        <v>26</v>
-      </c>
-      <c r="F63" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="30" t="s">
+      <c r="B63" s="60">
+        <v>9</v>
+      </c>
+      <c r="C63" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D63" s="60">
+        <v>26</v>
+      </c>
+      <c r="E63" s="60">
+        <v>26</v>
+      </c>
+      <c r="F63" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="B64" s="31">
-        <v>8</v>
-      </c>
-      <c r="C64" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D64" s="31">
-        <v>26</v>
-      </c>
-      <c r="E64" s="31">
-        <v>26</v>
-      </c>
-      <c r="F64" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="30" t="s">
+      <c r="B64" s="60">
+        <v>9</v>
+      </c>
+      <c r="C64" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D64" s="60">
+        <v>26</v>
+      </c>
+      <c r="E64" s="60">
+        <v>26</v>
+      </c>
+      <c r="F64" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="B65" s="31">
-        <v>8</v>
-      </c>
-      <c r="C65" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D65" s="31">
-        <v>26</v>
-      </c>
-      <c r="E65" s="31">
-        <v>26</v>
-      </c>
-      <c r="F65" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="30" t="s">
+      <c r="B65" s="60">
+        <v>9</v>
+      </c>
+      <c r="C65" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D65" s="60">
+        <v>26</v>
+      </c>
+      <c r="E65" s="60">
+        <v>26</v>
+      </c>
+      <c r="F65" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="59" t="s">
         <v>162</v>
       </c>
-      <c r="B66" s="31">
-        <v>8</v>
-      </c>
-      <c r="C66" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D66" s="31">
-        <v>26</v>
-      </c>
-      <c r="E66" s="31">
-        <v>26</v>
-      </c>
-      <c r="F66" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="30" t="s">
+      <c r="B66" s="60">
+        <v>9</v>
+      </c>
+      <c r="C66" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D66" s="60">
+        <v>26</v>
+      </c>
+      <c r="E66" s="60">
+        <v>26</v>
+      </c>
+      <c r="F66" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="B67" s="31">
-        <v>8</v>
-      </c>
-      <c r="C67" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D67" s="31">
-        <v>26</v>
-      </c>
-      <c r="E67" s="31">
-        <v>26</v>
-      </c>
-      <c r="F67" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="30" t="s">
+      <c r="B67" s="60">
+        <v>9</v>
+      </c>
+      <c r="C67" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D67" s="60">
+        <v>26</v>
+      </c>
+      <c r="E67" s="60">
+        <v>26</v>
+      </c>
+      <c r="F67" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="B68" s="31">
-        <v>8</v>
-      </c>
-      <c r="C68" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D68" s="31">
-        <v>26</v>
-      </c>
-      <c r="E68" s="31">
-        <v>26</v>
-      </c>
-      <c r="F68" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="30" t="s">
+      <c r="B68" s="60">
+        <v>9</v>
+      </c>
+      <c r="C68" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D68" s="60">
+        <v>26</v>
+      </c>
+      <c r="E68" s="60">
+        <v>26</v>
+      </c>
+      <c r="F68" s="60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="59" t="s">
         <v>164</v>
       </c>
-      <c r="B69" s="31">
-        <v>8</v>
-      </c>
-      <c r="C69" s="31">
-        <v>2022</v>
-      </c>
-      <c r="D69" s="31">
-        <v>26</v>
-      </c>
-      <c r="E69" s="31">
-        <v>26</v>
-      </c>
-      <c r="F69" s="31">
+      <c r="B69" s="60">
+        <v>9</v>
+      </c>
+      <c r="C69" s="60">
+        <v>2022</v>
+      </c>
+      <c r="D69" s="60">
+        <v>26</v>
+      </c>
+      <c r="E69" s="60">
+        <v>26</v>
+      </c>
+      <c r="F69" s="60">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A76" s="28"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="36"/>
     </row>
     <row r="77" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A77" s="29"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
+      <c r="A77" s="38"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
     </row>
     <row r="78" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A78" s="29"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
+      <c r="A78" s="38"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="36"/>
     </row>
     <row r="79" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A79" s="29"/>
-      <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
+      <c r="A79" s="38"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="36"/>
     </row>
     <row r="80" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A80" s="29"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
+      <c r="A80" s="38"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="36"/>
+      <c r="F80" s="36"/>
     </row>
     <row r="81" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A81" s="29"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
+      <c r="A81" s="38"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="36"/>
     </row>
     <row r="82" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A82" s="28"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
+      <c r="A82" s="37"/>
+      <c r="B82" s="36"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -5991,63 +6099,1930 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B109BBE4-4C0E-4B4D-94EC-BA18A18CC5DE}">
+  <dimension ref="A1:L46"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.81640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="9.7265625" customWidth="1"/>
+    <col min="4" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" customWidth="1"/>
+    <col min="9" max="9" width="24.453125" customWidth="1"/>
+    <col min="10" max="10" width="27.7265625" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="47">
+        <v>9</v>
+      </c>
+      <c r="C2" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="47">
+        <v>26</v>
+      </c>
+      <c r="E2" s="47">
+        <v>26</v>
+      </c>
+      <c r="F2" s="47">
+        <v>0</v>
+      </c>
+      <c r="G2" s="48">
+        <v>2</v>
+      </c>
+      <c r="H2" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="47">
+        <v>9</v>
+      </c>
+      <c r="C3" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D3" s="47">
+        <v>26</v>
+      </c>
+      <c r="E3" s="47">
+        <v>26</v>
+      </c>
+      <c r="F3" s="47">
+        <v>0</v>
+      </c>
+      <c r="G3" s="48">
+        <v>3</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="54" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="47">
+        <v>9</v>
+      </c>
+      <c r="C4" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D4" s="47">
+        <v>26</v>
+      </c>
+      <c r="E4" s="47">
+        <v>26</v>
+      </c>
+      <c r="F4" s="47">
+        <v>0</v>
+      </c>
+      <c r="G4" s="48">
+        <v>4</v>
+      </c>
+      <c r="H4" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="54" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="47">
+        <v>9</v>
+      </c>
+      <c r="C5" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D5" s="47">
+        <v>26</v>
+      </c>
+      <c r="E5" s="47">
+        <v>26</v>
+      </c>
+      <c r="F5" s="47">
+        <v>0</v>
+      </c>
+      <c r="G5" s="48">
+        <v>7</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="47">
+        <v>9</v>
+      </c>
+      <c r="C6" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D6" s="47">
+        <v>26</v>
+      </c>
+      <c r="E6" s="47">
+        <v>26</v>
+      </c>
+      <c r="F6" s="47">
+        <v>0</v>
+      </c>
+      <c r="G6" s="48">
+        <v>8</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="K6" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="L6" s="50"/>
+    </row>
+    <row r="7" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="47">
+        <v>9</v>
+      </c>
+      <c r="C7" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D7" s="47">
+        <v>26</v>
+      </c>
+      <c r="E7" s="47">
+        <v>26</v>
+      </c>
+      <c r="F7" s="47">
+        <v>0</v>
+      </c>
+      <c r="G7" s="48">
+        <v>10</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="54" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="47">
+        <v>9</v>
+      </c>
+      <c r="C8" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D8" s="47">
+        <v>26</v>
+      </c>
+      <c r="E8" s="47">
+        <v>26</v>
+      </c>
+      <c r="F8" s="47">
+        <v>0</v>
+      </c>
+      <c r="G8" s="48">
+        <v>12</v>
+      </c>
+      <c r="H8" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="54" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="47">
+        <v>9</v>
+      </c>
+      <c r="C9" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="47">
+        <v>26</v>
+      </c>
+      <c r="E9" s="47">
+        <v>26</v>
+      </c>
+      <c r="F9" s="47">
+        <v>0</v>
+      </c>
+      <c r="G9" s="48">
+        <v>14</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="54" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="47">
+        <v>9</v>
+      </c>
+      <c r="C10" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D10" s="47">
+        <v>26</v>
+      </c>
+      <c r="E10" s="47">
+        <v>26</v>
+      </c>
+      <c r="F10" s="47">
+        <v>0</v>
+      </c>
+      <c r="G10" s="48">
+        <v>15</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="K10" s="54" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="47">
+        <v>9</v>
+      </c>
+      <c r="C11" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D11" s="47">
+        <v>26</v>
+      </c>
+      <c r="E11" s="47">
+        <v>26</v>
+      </c>
+      <c r="F11" s="47">
+        <v>0</v>
+      </c>
+      <c r="G11" s="48">
+        <v>16</v>
+      </c>
+      <c r="H11" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" s="47">
+        <v>9</v>
+      </c>
+      <c r="C12" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D12" s="47">
+        <v>26</v>
+      </c>
+      <c r="E12" s="47">
+        <v>26</v>
+      </c>
+      <c r="F12" s="47">
+        <v>0</v>
+      </c>
+      <c r="G12" s="48">
+        <v>22</v>
+      </c>
+      <c r="H12" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="I12" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="K12" s="54" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" s="47">
+        <v>9</v>
+      </c>
+      <c r="C13" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D13" s="47">
+        <v>26</v>
+      </c>
+      <c r="E13" s="47">
+        <v>26</v>
+      </c>
+      <c r="F13" s="47">
+        <v>0</v>
+      </c>
+      <c r="G13" s="48">
+        <v>23</v>
+      </c>
+      <c r="H13" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="54" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" s="47">
+        <v>9</v>
+      </c>
+      <c r="C14" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D14" s="47">
+        <v>26</v>
+      </c>
+      <c r="E14" s="47">
+        <v>26</v>
+      </c>
+      <c r="F14" s="47">
+        <v>0</v>
+      </c>
+      <c r="G14" s="48">
+        <v>32</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="K14" s="50" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="47">
+        <v>9</v>
+      </c>
+      <c r="C15" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D15" s="47">
+        <v>26</v>
+      </c>
+      <c r="E15" s="47">
+        <v>26</v>
+      </c>
+      <c r="F15" s="47">
+        <v>0</v>
+      </c>
+      <c r="G15" s="48">
+        <v>33</v>
+      </c>
+      <c r="H15" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="50" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="47">
+        <v>9</v>
+      </c>
+      <c r="C16" s="40">
+        <v>2022</v>
+      </c>
+      <c r="D16" s="40">
+        <v>26</v>
+      </c>
+      <c r="E16" s="40">
+        <v>26</v>
+      </c>
+      <c r="F16" s="40">
+        <v>0</v>
+      </c>
+      <c r="G16" s="41">
+        <v>34</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="47">
+        <v>9</v>
+      </c>
+      <c r="C17" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D17" s="47">
+        <v>26</v>
+      </c>
+      <c r="E17" s="47">
+        <v>26</v>
+      </c>
+      <c r="F17" s="47">
+        <v>0</v>
+      </c>
+      <c r="G17" s="48">
+        <v>39</v>
+      </c>
+      <c r="H17" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="K17" s="50" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="47">
+        <v>9</v>
+      </c>
+      <c r="C18" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D18" s="47">
+        <v>26</v>
+      </c>
+      <c r="E18" s="47">
+        <v>26</v>
+      </c>
+      <c r="F18" s="47">
+        <v>0</v>
+      </c>
+      <c r="G18" s="48">
+        <v>41</v>
+      </c>
+      <c r="H18" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" s="50" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="B19" s="47">
+        <v>9</v>
+      </c>
+      <c r="C19" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D19" s="47">
+        <v>26</v>
+      </c>
+      <c r="E19" s="47">
+        <v>26</v>
+      </c>
+      <c r="F19" s="47">
+        <v>0</v>
+      </c>
+      <c r="G19" s="48">
+        <v>42</v>
+      </c>
+      <c r="H19" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" s="50" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="47">
+        <v>9</v>
+      </c>
+      <c r="C20" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D20" s="47">
+        <v>26</v>
+      </c>
+      <c r="E20" s="47">
+        <v>26</v>
+      </c>
+      <c r="F20" s="47">
+        <v>0</v>
+      </c>
+      <c r="G20" s="48">
+        <v>46</v>
+      </c>
+      <c r="H20" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="I20" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" s="50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="47">
+        <v>9</v>
+      </c>
+      <c r="C21" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D21" s="47">
+        <v>26</v>
+      </c>
+      <c r="E21" s="47">
+        <v>26</v>
+      </c>
+      <c r="F21" s="47">
+        <v>0</v>
+      </c>
+      <c r="G21" s="48">
+        <v>49</v>
+      </c>
+      <c r="H21" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="47">
+        <v>9</v>
+      </c>
+      <c r="C22" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D22" s="47">
+        <v>26</v>
+      </c>
+      <c r="E22" s="47">
+        <v>26</v>
+      </c>
+      <c r="F22" s="47">
+        <v>0</v>
+      </c>
+      <c r="G22" s="48">
+        <v>52</v>
+      </c>
+      <c r="H22" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="I22" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" s="50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23" s="47">
+        <v>9</v>
+      </c>
+      <c r="C23" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D23" s="47">
+        <v>26</v>
+      </c>
+      <c r="E23" s="47">
+        <v>26</v>
+      </c>
+      <c r="F23" s="47">
+        <v>0</v>
+      </c>
+      <c r="G23" s="48">
+        <v>54</v>
+      </c>
+      <c r="H23" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="L23" s="56"/>
+    </row>
+    <row r="24" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" s="47">
+        <v>9</v>
+      </c>
+      <c r="C24" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D24" s="47">
+        <v>26</v>
+      </c>
+      <c r="E24" s="47">
+        <v>26</v>
+      </c>
+      <c r="F24" s="47">
+        <v>0</v>
+      </c>
+      <c r="G24" s="48">
+        <v>55</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="B25" s="47">
+        <v>9</v>
+      </c>
+      <c r="C25" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D25" s="47">
+        <v>26</v>
+      </c>
+      <c r="E25" s="47">
+        <v>26</v>
+      </c>
+      <c r="F25" s="47">
+        <v>0</v>
+      </c>
+      <c r="G25" s="48">
+        <v>56</v>
+      </c>
+      <c r="H25" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="K25" s="50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="47">
+        <v>9</v>
+      </c>
+      <c r="C26" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="47">
+        <v>26</v>
+      </c>
+      <c r="E26" s="47">
+        <v>26</v>
+      </c>
+      <c r="F26" s="47">
+        <v>0</v>
+      </c>
+      <c r="G26" s="48">
+        <v>57</v>
+      </c>
+      <c r="H26" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="K26" s="50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="47">
+        <v>9</v>
+      </c>
+      <c r="C27" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D27" s="47">
+        <v>26</v>
+      </c>
+      <c r="E27" s="47">
+        <v>26</v>
+      </c>
+      <c r="F27" s="47">
+        <v>0</v>
+      </c>
+      <c r="G27" s="48">
+        <v>58</v>
+      </c>
+      <c r="H27" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" s="50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="47">
+        <v>9</v>
+      </c>
+      <c r="C28" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D28" s="47">
+        <v>26</v>
+      </c>
+      <c r="E28" s="47">
+        <v>26</v>
+      </c>
+      <c r="F28" s="47">
+        <v>0</v>
+      </c>
+      <c r="G28" s="48">
+        <v>59</v>
+      </c>
+      <c r="H28" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="K28" s="50" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29" s="47">
+        <v>9</v>
+      </c>
+      <c r="C29" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D29" s="47">
+        <v>26</v>
+      </c>
+      <c r="E29" s="47">
+        <v>26</v>
+      </c>
+      <c r="F29" s="47">
+        <v>0</v>
+      </c>
+      <c r="G29" s="48">
+        <v>62</v>
+      </c>
+      <c r="H29" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="I29" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="50" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="47">
+        <v>9</v>
+      </c>
+      <c r="C30" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D30" s="47">
+        <v>26</v>
+      </c>
+      <c r="E30" s="47">
+        <v>26</v>
+      </c>
+      <c r="F30" s="47">
+        <v>0</v>
+      </c>
+      <c r="G30" s="48">
+        <v>63</v>
+      </c>
+      <c r="H30" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="I30" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="50" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" s="47">
+        <v>9</v>
+      </c>
+      <c r="C31" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D31" s="47">
+        <v>26</v>
+      </c>
+      <c r="E31" s="47">
+        <v>26</v>
+      </c>
+      <c r="F31" s="47">
+        <v>0</v>
+      </c>
+      <c r="G31" s="48">
+        <v>65</v>
+      </c>
+      <c r="H31" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="50" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="47">
+        <v>9</v>
+      </c>
+      <c r="C32" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D32" s="47">
+        <v>26</v>
+      </c>
+      <c r="E32" s="47">
+        <v>26</v>
+      </c>
+      <c r="F32" s="47">
+        <v>0</v>
+      </c>
+      <c r="G32" s="48">
+        <v>66</v>
+      </c>
+      <c r="H32" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J32" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="K32" s="50" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="47">
+        <v>9</v>
+      </c>
+      <c r="C33" s="47">
+        <v>2022</v>
+      </c>
+      <c r="D33" s="47">
+        <v>26</v>
+      </c>
+      <c r="E33" s="47">
+        <v>26</v>
+      </c>
+      <c r="F33" s="47">
+        <v>0</v>
+      </c>
+      <c r="G33" s="48">
+        <v>68</v>
+      </c>
+      <c r="H33" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="I33" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="J33" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="K33" s="50" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H36">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H37">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H38">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H39">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A40" s="37"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="H40">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A41" s="38"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="H41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A42" s="38"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="H42">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A43" s="38"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+    </row>
+    <row r="44" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A44" s="38"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="H44">
+        <f>SUM(H36:H42)</f>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A45" s="38"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="H45" s="45">
+        <f>H44/7</f>
+        <v>81.142857142857139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A46" s="37"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE0CADD8-1F8D-4423-BE8A-07ABED74AB3B}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView topLeftCell="C2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.81640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="9.7265625" customWidth="1"/>
+    <col min="4" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" customWidth="1"/>
+    <col min="9" max="9" width="24.453125" customWidth="1"/>
+    <col min="10" max="10" width="27.7265625" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="68" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+    </row>
+    <row r="2" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="28">
+        <v>7</v>
+      </c>
+      <c r="C2" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="28">
+        <v>25</v>
+      </c>
+      <c r="E2" s="28">
+        <v>25</v>
+      </c>
+      <c r="F2" s="28">
+        <v>0</v>
+      </c>
+      <c r="G2" s="29">
+        <v>1</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="28">
+        <v>7</v>
+      </c>
+      <c r="C3" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D3" s="28">
+        <v>25</v>
+      </c>
+      <c r="E3" s="28">
+        <v>25</v>
+      </c>
+      <c r="F3" s="28">
+        <v>0</v>
+      </c>
+      <c r="G3" s="29">
+        <v>2</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="28">
+        <v>7</v>
+      </c>
+      <c r="C4" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D4" s="28">
+        <v>25</v>
+      </c>
+      <c r="E4" s="28">
+        <v>25</v>
+      </c>
+      <c r="F4" s="28">
+        <v>0</v>
+      </c>
+      <c r="G4" s="29">
+        <v>3</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="28">
+        <v>7</v>
+      </c>
+      <c r="C5" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D5" s="28">
+        <v>25</v>
+      </c>
+      <c r="E5" s="28">
+        <v>25</v>
+      </c>
+      <c r="F5" s="28">
+        <v>0</v>
+      </c>
+      <c r="G5" s="29">
+        <v>4</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="28">
+        <v>7</v>
+      </c>
+      <c r="C6" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D6" s="28">
+        <v>25</v>
+      </c>
+      <c r="E6" s="28">
+        <v>25</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0</v>
+      </c>
+      <c r="G6" s="29">
+        <v>5</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="28">
+        <v>7</v>
+      </c>
+      <c r="C7" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D7" s="28">
+        <v>25</v>
+      </c>
+      <c r="E7" s="28">
+        <v>25</v>
+      </c>
+      <c r="F7" s="28">
+        <v>0</v>
+      </c>
+      <c r="G7" s="29">
+        <v>6</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="28">
+        <v>7</v>
+      </c>
+      <c r="C8" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D8" s="28">
+        <v>25</v>
+      </c>
+      <c r="E8" s="28">
+        <v>25</v>
+      </c>
+      <c r="F8" s="28">
+        <v>0</v>
+      </c>
+      <c r="G8" s="29">
+        <v>7</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="28">
+        <v>7</v>
+      </c>
+      <c r="C9" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="28">
+        <v>25</v>
+      </c>
+      <c r="E9" s="28">
+        <v>25</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29">
+        <v>8</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="28">
+        <v>7</v>
+      </c>
+      <c r="C10" s="28">
+        <v>2022</v>
+      </c>
+      <c r="D10" s="28">
+        <v>25</v>
+      </c>
+      <c r="E10" s="28">
+        <v>25</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0</v>
+      </c>
+      <c r="G10" s="29">
+        <v>9</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G13" s="2">
+        <v>2</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A14" s="37"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="2">
+        <v>3</v>
+      </c>
+      <c r="H14" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="I14" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A15" s="38"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="2">
+        <v>4</v>
+      </c>
+      <c r="H15" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+      <c r="A16" s="38"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="21" x14ac:dyDescent="0.5">
+      <c r="A17" s="38"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="2">
+        <v>6</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.5">
+      <c r="A18" s="38"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="2">
+        <v>7</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="42" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="21" x14ac:dyDescent="0.5">
+      <c r="A19" s="37"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="2">
+        <v>8</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G20" s="2">
+        <v>9</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G21" s="2">
+        <v>10</v>
+      </c>
+      <c r="H21" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G22" s="2">
+        <v>11</v>
+      </c>
+      <c r="H22" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G23" s="2">
+        <v>12</v>
+      </c>
+      <c r="H23" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="I23" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G24" s="2">
+        <v>13</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G25" s="2">
+        <v>14</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="I25" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4802CEB9-E954-45DE-9902-73EBC6E635B2}">
   <dimension ref="A4:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="B5" s="28"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="B6" s="29"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="B7" s="29"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="B8" s="29"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="B9" s="29"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>